<commit_message>
Add new data dictionary
Attached is a new data dictionary.  I have made the requested edits to the survey so there are now additional variables corresponding to each component of the score, and the value of these variables will be the value that is added to the score by the algorithm at the end of the MOCA.  I’ve also added variables to capture the date/time the MOCA is started, as well as the date and day of the week that the score is calculated.  In the attached spreadsheet, I’ve highlighted green in column A those rows which are new additions.  These changes are effective today 2/7/23 at 3:48 PM Eastern.
</commit_message>
<xml_diff>
--- a/codebook/1833_DETECT_DataDictionary.xlsx
+++ b/codebook/1833_DETECT_DataDictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Projects_Active\Proj1833 Univ TX MedStar\Tasks\Set up\Survey\Data dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443DBB70-49AB-4734-9CE6-E07ECC2A0539}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFE0A1B-9BCB-4921-9B9B-59EBD5E840B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="tblDictionary" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tblDictionary!$A$1:$C$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tblDictionary!$A$1:$D$80</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="195">
   <si>
     <t>Variable</t>
   </si>
@@ -697,10 +697,6 @@
     <t>MOCA_DELREC</t>
   </si>
   <si>
-    <t>I read some words to you earlier, which I asked you to remember. Tell me as many of those words as you can remember.    [NOTE: Make a check mark for each of the words correctly recalled spontaneously without any cues, in the allocated space]    FACE - VELVET - CHURCH - DAISY - RED
-Format = numeric string containing all choices correctly recalled.  e.g. "235" means Velvet, Church, and Red were correctly recalled.</t>
-  </si>
-  <si>
     <t>OR_PLACECITY</t>
   </si>
   <si>
@@ -710,13 +706,208 @@
   <si>
     <t>Now, tell me the name of the place you are in, and which city it is in.    [INTERVIEWER, check the box for each item which is correct.  For the place, any reasonable answer should be deemed correct, e.g. my living room, my house, the store, etc.  Answers such as "on a spaceship" or "I don't know" are incorrect.  For the city, it is correct if it matches the city listed below.  Again "I don't know" is incorrect.]    Correct City:  [CITY]
 Format = numeric string containing all choices correctly recalled.  e.g. "12" means both place and city were correctly provided.</t>
+  </si>
+  <si>
+    <t>Contribution to Score</t>
+  </si>
+  <si>
+    <t>The value of this variable gets added to the score.  So the addition will be either "0" or "1".  (a value of 9 would mean the call ended)</t>
+  </si>
+  <si>
+    <t>The value of this variable is the number of subtractions that were correct. So it will be a whole number between 0 and 5.  The formula that calculates the score will add to the score based on the following schema:
+SERIAL_SCORE value of 0 = 0 added to score
+SERIAL_SCORE value of 1 = 1 added to score
+SERIAL_SCORE value of 2 or 3 = 2 added to score
+SERIAL_SCORE value of 4 or 5 = 3 added to score</t>
+  </si>
+  <si>
+    <t>The value of this variable gets added to the score.  So the addition will be either 0, 1, or 2.  (a value of 9 would mean the call ended)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The number of </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>digits</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in this variable's numeric value gets added to the score.  So, a value of 215 would mean "3" gets added to the score.  A value of 34 would mean "2" gets added to the score.  Etc.</t>
+    </r>
+  </si>
+  <si>
+    <t>I read some words to you earlier, which I asked you to remember. Tell me as many of those words as you can remember.    [NOTE: Make a check mark for each of the words correctly recalled spontaneously without any cues, in the allocated space]    FACE - VELVET - CHURCH - DAISY - RED
+Format = numeric string containing all choices correctly recalled.  e.g. "235" means Velvet, Church, and Red were correctly recalled.
+Note:  the digits representing the answer codes can appear in any order based on the order in which the interviewer clicks the choices.  So "235" could also be "325"  or "523" etc.</t>
+  </si>
+  <si>
+    <t>This variable represents 3 separate contributions to the score:  Year, Month, and Date.  Each part individually is compared to the corresponding date part in the "ResLastCallDate" variable.  For each part that matches, a value of 1 is added to the score.  So from this variable any value between 0 and 3 could be added to the score.  For example, if the first four digits of this variable (year) matches the first four digits of "ResLastCallDate" then 1 is added to the score, otherwise 0 is added to the score.  Next the 5th/6th digits (month), and 7th/8th digits (date) are compared with "ResLastCallDate" in similar fashion, each time with either a 0 or a 1 being added to the score.</t>
+  </si>
+  <si>
+    <t>From this variable, either a 0 or 1 is added to the score, based on whether the day of the week provided by the respondent matches the current day of the week at the time of the interview.  Unfortunately, this is compared on the back-end using a formula which converts the current date (back-end system variable) to a coded numeric value for the current weekday, and that value is not represented in the exported data.  OR_DAY has been set up with the same codes representing each day, so once an answer is provided, is it compared to the computed current weekday and if it matches then "1" is added to the score, otherwise "0" is added to the score.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The number of </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>digits</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in this variable's numeric value gets added to the score.  So, a value of "12" or "21" means 2 gets added to the score.  A value of "1" or "2" means 1 gets added to the score.  An empty cell means 0 gets added to the score.</t>
+    </r>
+  </si>
+  <si>
+    <t>This is the final score, calculated based on all of the variables highlighted here in yellow:
+MOCA_DIGFORW
+MOCA_DIGBACK
+MOCA_VIGIL
+SERIAL_SCORE
+MOCA_SENTREP
+MOCA_VERBFLU
+MOCA_ABSTRAC
+MOCA_DELREC
+OR_DATE
+OR_DAY
+OR_PLACECITY</t>
+  </si>
+  <si>
+    <t>DATEMOCASTRT</t>
+  </si>
+  <si>
+    <t>TIMEMOCASTRT</t>
+  </si>
+  <si>
+    <t>Date respondent began MOCA "yyyyMMdd" format</t>
+  </si>
+  <si>
+    <t>Time respondent began MOCA "HHmm" format</t>
+  </si>
+  <si>
+    <t>SCORE_DIGFOR</t>
+  </si>
+  <si>
+    <t>SCORE_DIGBAK</t>
+  </si>
+  <si>
+    <t>SCORE_VIGIL</t>
+  </si>
+  <si>
+    <t>SCORE_SERIAL</t>
+  </si>
+  <si>
+    <t>SCORE_SNTREP</t>
+  </si>
+  <si>
+    <t>SCORE_VRBFLU</t>
+  </si>
+  <si>
+    <t>SCORE_ABSTRC</t>
+  </si>
+  <si>
+    <t>SCORE_DELREC</t>
+  </si>
+  <si>
+    <t>SCORE_YEAR</t>
+  </si>
+  <si>
+    <t>SCORE_MONTH</t>
+  </si>
+  <si>
+    <t>SCORE_DATE</t>
+  </si>
+  <si>
+    <t>SCORE_DAY</t>
+  </si>
+  <si>
+    <t>SCORE_PLCCTY</t>
+  </si>
+  <si>
+    <t>DATEOFSCORE</t>
+  </si>
+  <si>
+    <t>DAYOFSCORE</t>
+  </si>
+  <si>
+    <t>Date SCORE was calculated "yyyyMMdd" format</t>
+  </si>
+  <si>
+    <t>Day of week SCORE was calculated</t>
+  </si>
+  <si>
+    <t>Value added to SCORE based on MOCA_DIGFORW</t>
+  </si>
+  <si>
+    <t>Value added to SCORE based on MOCA_DIGBACK</t>
+  </si>
+  <si>
+    <t>Value added to SCORE based on MOCA_VIGIL</t>
+  </si>
+  <si>
+    <t>Value added to SCORE based on MOCA_SERIAL1 through MOCA_SERIAL5</t>
+  </si>
+  <si>
+    <t>Value added to SCORE based on MOCA_SENTREP</t>
+  </si>
+  <si>
+    <t>Value added to SCORE based on MOCA_VERBFLU</t>
+  </si>
+  <si>
+    <t>Value added to SCORE based on MOCA_ABSTRAC</t>
+  </si>
+  <si>
+    <t>Value added to SCORE based on MOCA_DELREC</t>
+  </si>
+  <si>
+    <t>Value added to SCORE based on "year" portion of OR_DATE</t>
+  </si>
+  <si>
+    <t>Value added to SCORE based on  "month" portion of OR_DATE</t>
+  </si>
+  <si>
+    <t>Value added to SCORE based on  "date" portion of OR_DATE</t>
+  </si>
+  <si>
+    <t>Value added to SCORE based on OR_DAY</t>
+  </si>
+  <si>
+    <t>Value added to SCORE based on OR_PLACECITY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -745,8 +936,22 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -771,8 +976,26 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -795,11 +1018,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -814,6 +1048,33 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1154,7 +1415,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1166,9 +1427,10 @@
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="124.28515625" customWidth="1"/>
     <col min="3" max="3" width="52.28515625" customWidth="1"/>
+    <col min="4" max="4" width="70.42578125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1178,8 +1440,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>120</v>
       </c>
@@ -1189,8 +1454,9 @@
       <c r="C2" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>121</v>
       </c>
@@ -1200,9 +1466,10 @@
       <c r="C3" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>122</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1211,8 +1478,9 @@
       <c r="C4" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>123</v>
       </c>
@@ -1222,8 +1490,9 @@
       <c r="C5" s="4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>124</v>
       </c>
@@ -1233,8 +1502,9 @@
       <c r="C6" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -1244,8 +1514,9 @@
       <c r="C7" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>126</v>
       </c>
@@ -1255,8 +1526,9 @@
       <c r="C8" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>127</v>
       </c>
@@ -1266,8 +1538,9 @@
       <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>128</v>
       </c>
@@ -1277,8 +1550,9 @@
       <c r="C10" s="4" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>129</v>
       </c>
@@ -1288,8 +1562,9 @@
       <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -1299,8 +1574,9 @@
       <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
@@ -1310,8 +1586,9 @@
       <c r="C13" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -1321,8 +1598,9 @@
       <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -1332,8 +1610,9 @@
       <c r="C15" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1343,8 +1622,9 @@
       <c r="C16" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1354,8 +1634,9 @@
       <c r="C17" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -1365,8 +1646,9 @@
       <c r="C18" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1376,8 +1658,9 @@
       <c r="C19" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
@@ -1387,8 +1670,9 @@
       <c r="C20" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -1398,8 +1682,9 @@
       <c r="C21" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1409,8 +1694,9 @@
       <c r="C22" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -1420,8 +1706,9 @@
       <c r="C23" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
@@ -1431,8 +1718,9 @@
       <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>31</v>
       </c>
@@ -1442,8 +1730,9 @@
       <c r="C25" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>33</v>
       </c>
@@ -1453,8 +1742,9 @@
       <c r="C26" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>35</v>
       </c>
@@ -1464,8 +1754,9 @@
       <c r="C27" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>36</v>
       </c>
@@ -1475,8 +1766,9 @@
       <c r="C28" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
@@ -1486,8 +1778,9 @@
       <c r="C29" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>39</v>
       </c>
@@ -1497,8 +1790,9 @@
       <c r="C30" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>42</v>
       </c>
@@ -1508,8 +1802,9 @@
       <c r="C31" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="D31" s="9"/>
+    </row>
+    <row r="32" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>45</v>
       </c>
@@ -1519,8 +1814,9 @@
       <c r="C32" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D32" s="9"/>
+    </row>
+    <row r="33" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>48</v>
       </c>
@@ -1530,8 +1826,9 @@
       <c r="C33" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>51</v>
       </c>
@@ -1541,8 +1838,9 @@
       <c r="C34" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>54</v>
       </c>
@@ -1552,8 +1850,9 @@
       <c r="C35" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D35" s="9"/>
+    </row>
+    <row r="36" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>56</v>
       </c>
@@ -1563,8 +1862,9 @@
       <c r="C36" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D36" s="9"/>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>59</v>
       </c>
@@ -1574,8 +1874,9 @@
       <c r="C37" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="D37" s="9"/>
+    </row>
+    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>62</v>
       </c>
@@ -1585,8 +1886,9 @@
       <c r="C38" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="D38" s="9"/>
+    </row>
+    <row r="39" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>145</v>
       </c>
@@ -1596,8 +1898,9 @@
       <c r="C39" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D39" s="9"/>
+    </row>
+    <row r="40" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>143</v>
       </c>
@@ -1607,262 +1910,515 @@
       <c r="C40" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="D40" s="9"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" s="9"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="9"/>
+    </row>
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="D43" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="D44" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="D45" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="C46" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D46" s="9"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="C47" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D47" s="9"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="C48" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48" s="9"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="C49" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" s="9"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B50" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="C50" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D50" s="9"/>
+    </row>
+    <row r="51" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="C51" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="D52" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B53" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="D53" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+      <c r="D54" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A55" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B55" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A58" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C55" s="4" t="s">
+      <c r="B58" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D59" s="9"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D60" s="9"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D61" s="9"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D62" s="9"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D63" s="9"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D64" s="9"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D65" s="9"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D66" s="9"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D67" s="9"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D68" s="9"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D69" s="9"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D70" s="9"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D71" s="9"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D72" s="9"/>
+    </row>
+    <row r="73" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A73" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+      <c r="D73" s="9"/>
+    </row>
+    <row r="74" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B74" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C74" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+      <c r="D74" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C75" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+      <c r="D75" s="9"/>
+    </row>
+    <row r="76" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C76" s="3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+      <c r="D76" s="9"/>
+    </row>
+    <row r="77" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C77" s="3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+      <c r="D77" s="9"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B78" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C78" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+      <c r="D78" s="9"/>
+    </row>
+    <row r="79" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B79" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C79" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+      <c r="D79" s="9"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B80" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C80" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D80" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C63" xr:uid="{BF9C88D4-835D-42FD-88FA-0BB656300E39}"/>
+  <autoFilter ref="A1:D80" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>